<commit_message>
Figure edits before reorganization
</commit_message>
<xml_diff>
--- a/submission/table_S7_PERMANOVA_dn1_source.xlsx
+++ b/submission/table_S7_PERMANOVA_dn1_source.xlsx
@@ -414,7 +414,7 @@
         <v>0.6165614048558912</v>
       </c>
       <c r="C4">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -432,7 +432,7 @@
         <v>0.3335414119116302</v>
       </c>
       <c r="C5">
-        <v>0.027</v>
+        <v>0.02</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
         <v>0.1361110669582063</v>
       </c>
       <c r="C10">
-        <v>0.601</v>
+        <v>0.595</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -540,7 +540,7 @@
         <v>0.1014554865924366</v>
       </c>
       <c r="C11">
-        <v>0.949</v>
+        <v>0.965</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -558,7 +558,7 @@
         <v>0.3401942363375496</v>
       </c>
       <c r="C12">
-        <v>0.145</v>
+        <v>0.13</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -576,7 +576,7 @@
         <v>0.242822145258084</v>
       </c>
       <c r="C13">
-        <v>0.486</v>
+        <v>0.474</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>

</xml_diff>